<commit_message>
Se actualiza DataTable previo a la ejecucion
</commit_message>
<xml_diff>
--- a/Default.xlsx
+++ b/Default.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="2_FlowBuyTicket" sheetId="3" r:id="rId3"/>
     <sheet name="3_LogOut" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="40001"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t/>
   </si>
@@ -43,9 +43,6 @@
     <t>TIPOCONEXION</t>
   </si>
   <si>
-    <t>Giovanna Guerra</t>
-  </si>
-  <si>
     <t>i_PasswordSecure</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>o_ValLoginName</t>
   </si>
   <si>
-    <t>Pablo Rodriguez</t>
-  </si>
-  <si>
     <t>maria</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t>Economy</t>
   </si>
   <si>
-    <t>Abraham Rivera</t>
-  </si>
-  <si>
     <t>San Francisco</t>
   </si>
   <si>
@@ -110,14 +101,22 @@
   </si>
   <si>
     <t>24-Feb-2024</t>
+  </si>
+  <si>
+    <t>Agus Dina</t>
+  </si>
+  <si>
+    <t>Ivan Damboriana</t>
+  </si>
+  <si>
+    <t>Gian Dina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="20">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,126 +140,6 @@
       <color indexed="12"/>
       <name val="Mic Shell Dlg"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,16 +188,16 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -334,6 +213,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -625,29 +506,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.1484375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.1484375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1">
-      <c t="s">
+    <row r="1" spans="1:3" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c t="s">
-        <v>24</v>
-      </c>
-      <c t="s">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -662,50 +544,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.1484375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.1484375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1">
-      <c t="s">
-        <v>11</v>
-      </c>
-      <c t="s">
+    <row r="1" spans="1:5" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c t="s">
-        <v>18</v>
-      </c>
-      <c t="s">
-        <v>14</v>
-      </c>
-      <c t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row s="2" customFormat="1">
-      <c s="7" t="s">
-        <v>20</v>
-      </c>
-      <c s="1" t="s">
-        <v>10</v>
-      </c>
-      <c s="3"/>
-      <c s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -720,127 +603,128 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1484375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.1484375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="5" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.1484375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1">
-      <c t="s">
+    <row r="1" spans="1:9" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c t="s">
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-      <c t="s">
-        <v>15</v>
-      </c>
-      <c t="s">
-        <v>4</v>
-      </c>
-      <c t="s">
-        <v>22</v>
-      </c>
-      <c t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c t="s">
-        <v>5</v>
-      </c>
-      <c t="s">
-        <v>17</v>
-      </c>
-      <c t="s">
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row s="2" customFormat="1">
-      <c s="1" t="s">
-        <v>28</v>
-      </c>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1" t="s">
-        <v>2</v>
-      </c>
-      <c s="1" t="s">
-        <v>21</v>
-      </c>
-      <c s="1">
-        <v>1</v>
-      </c>
-      <c s="1" t="s">
-        <v>27</v>
-      </c>
-      <c s="3"/>
-      <c s="3" t="s">
-        <v>0</v>
-      </c>
-      <c s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row s="2" customFormat="1">
-      <c s="1" t="s">
-        <v>28</v>
-      </c>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
-      <c s="1" t="s">
-        <v>13</v>
-      </c>
-      <c s="1">
-        <v>2</v>
-      </c>
-      <c s="1" t="s">
-        <v>19</v>
-      </c>
-      <c s="3"/>
-      <c s="3"/>
-      <c s="4"/>
-    </row>
-    <row s="2" customFormat="1">
-      <c s="1" t="s">
-        <v>28</v>
-      </c>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1" t="s">
-        <v>25</v>
-      </c>
-      <c s="1" t="s">
-        <v>26</v>
-      </c>
-      <c s="1">
-        <v>3</v>
-      </c>
-      <c s="1" t="s">
-        <v>8</v>
-      </c>
-      <c s="3"/>
-      <c s="3"/>
-      <c s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="4"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -853,25 +737,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" width="9.1484375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1">
-      <c t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row>
-      <c s="4" t="s">
+    <row r="1" spans="1:1" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>